<commit_message>
update instructions to reflect dir change
</commit_message>
<xml_diff>
--- a/excel_template/Fixation&ROI_template.xlsx
+++ b/excel_template/Fixation&ROI_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="225" windowWidth="9435" windowHeight="11640"/>
+    <workbookView xWindow="120" yWindow="285" windowWidth="9435" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="results.roi" sheetId="1" r:id="rId1"/>
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P244"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5:L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,7 +1132,7 @@
         <v>178</v>
       </c>
       <c r="L5" s="10" t="e">
-        <f>AVERAGEIF(F5:F250, "&gt;0")</f>
+        <f>AVERAGEIF(F5:F556, "&gt;0")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M5" s="32"/>
@@ -1153,7 +1153,7 @@
         <v>179</v>
       </c>
       <c r="L6" s="10" t="e">
-        <f>AVERAGEIF(G5:G250, "&gt;0")</f>
+        <f>AVERAGEIF(G5:G556, "&gt;0")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M6" s="12"/>
@@ -1174,7 +1174,7 @@
         <v>180</v>
       </c>
       <c r="L7" s="10" t="e">
-        <f>AVERAGEIF(H5:H250, "&gt;0")</f>
+        <f>AVERAGEIF(H5:H556, "&gt;0")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M7" s="12"/>
@@ -1195,7 +1195,7 @@
         <v>181</v>
       </c>
       <c r="L8" s="10" t="e">
-        <f>AVERAGEIF(I5:I250,"&gt;0")</f>
+        <f>AVERAGEIF(I5:I556,"&gt;0")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M8" s="12"/>
@@ -1216,7 +1216,7 @@
         <v>146</v>
       </c>
       <c r="L9" s="10" t="e">
-        <f>AVERAGEIFS(F5:F300, F5:F300, "&gt;0", C5:C300, "=1")</f>
+        <f>AVERAGEIFS(F5:F556, F5:F556, "&gt;0", C5:C556, "=1")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M9" s="12"/>
@@ -1237,7 +1237,7 @@
         <v>147</v>
       </c>
       <c r="L10" s="10" t="e">
-        <f>AVERAGEIFS(G5:G300, G5:G300, "&gt;0", C5:C300, "=1")</f>
+        <f>AVERAGEIFS(G5:G556, G5:G556, "&gt;0", C5:C556, "=1")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="32"/>
@@ -1258,7 +1258,7 @@
         <v>148</v>
       </c>
       <c r="L11" s="10" t="e">
-        <f>AVERAGEIFS(H5:H300, H5:H300, "&gt;0", C5:C300, "=1")</f>
+        <f>AVERAGEIFS(H5:H556, H5:H556, "&gt;0", C5:C556, "=1")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M11" s="12"/>
@@ -1279,7 +1279,7 @@
         <v>149</v>
       </c>
       <c r="L12" s="10" t="e">
-        <f>AVERAGEIFS(I5:I300, I5:I300, "&gt;0", C5:C300, "=1")</f>
+        <f>AVERAGEIFS(I5:I556, I5:I556, "&gt;0", C5:C556, "=1")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M12" s="12"/>
@@ -1300,7 +1300,7 @@
         <v>150</v>
       </c>
       <c r="L13" s="10" t="e">
-        <f>AVERAGEIFS(F5:F300, F5:F300, "&gt;0", C5:C300, "=2")</f>
+        <f>AVERAGEIFS(F5:F556, F5:F556, "&gt;0", C5:C556, "=2")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M13" s="12"/>
@@ -1321,7 +1321,7 @@
         <v>151</v>
       </c>
       <c r="L14" s="10" t="e">
-        <f>AVERAGEIFS(G5:G300, G5:G300, "&gt;0", C5:C300, "=2")</f>
+        <f>AVERAGEIFS(G5:G556, G5:G556, "&gt;0", C5:C556, "=2")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M14" s="12"/>
@@ -1342,7 +1342,7 @@
         <v>152</v>
       </c>
       <c r="L15" s="10" t="e">
-        <f>AVERAGEIFS(H5:H300, H5:H300, "&gt;0", C5:C300, "=2")</f>
+        <f>AVERAGEIFS(H5:H556, H5:H556, "&gt;0", C5:C556, "=2")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M15" s="32"/>
@@ -1363,7 +1363,7 @@
         <v>153</v>
       </c>
       <c r="L16" s="10" t="e">
-        <f>AVERAGEIFS(I5:I300, I5:I300, "&gt;0", C5:C300, "=2")</f>
+        <f>AVERAGEIFS(I5:I556, I5:I556, "&gt;0", C5:C556, "=2")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M16" s="12"/>
@@ -1384,7 +1384,7 @@
         <v>154</v>
       </c>
       <c r="L17" s="10" t="e">
-        <f>AVERAGEIFS(F5:F300, F5:F300, "&gt;0", C5:C300, "=1", D5:D300, "=1")</f>
+        <f>AVERAGEIFS(F5:F556, F5:F556, "&gt;0", C5:C556, "=1", D5:D556, "=1")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M17" s="12"/>
@@ -1405,7 +1405,7 @@
         <v>155</v>
       </c>
       <c r="L18" s="10" t="e">
-        <f>AVERAGEIFS(G5:G300, G5:G300, "&gt;0", C5:C300, "=1", D5:D300, "=1")</f>
+        <f>AVERAGEIFS(G5:G556, G5:G556, "&gt;0", C5:C556, "=1", D5:D556, "=1")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M18" s="12"/>
@@ -1426,7 +1426,7 @@
         <v>156</v>
       </c>
       <c r="L19" s="10" t="e">
-        <f>AVERAGEIFS(H5:H300, H5:H300, "&gt;0", C5:C300, "=1", D5:D300, "=1")</f>
+        <f>AVERAGEIFS(H5:H556, H5:H556, "&gt;0", C5:C556, "=1", D5:D556, "=1")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M19" s="12"/>
@@ -1447,7 +1447,7 @@
         <v>157</v>
       </c>
       <c r="L20" s="10" t="e">
-        <f>AVERAGEIFS(I5:I300, I5:I300, "&gt;0", C5:C300, "=1", D5:D300, "=1")</f>
+        <f>AVERAGEIFS(I5:I556, I5:I556, "&gt;0", C5:C556, "=1", D5:D556, "=1")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M20" s="32"/>
@@ -1468,7 +1468,7 @@
         <v>177</v>
       </c>
       <c r="L21" s="10" t="e">
-        <f>AVERAGEIFS(F5:F300, F5:F300, "&gt;0", C5:C300, "=2", D5:D300, "=1")</f>
+        <f>AVERAGEIFS(F5:F556, F5:F556, "&gt;0", C5:C556, "=2", D5:D556, "=1")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M21" s="12"/>
@@ -1489,7 +1489,7 @@
         <v>176</v>
       </c>
       <c r="L22" s="10" t="e">
-        <f>AVERAGEIFS(G5:G300, G5:G300, "&gt;0", C5:C300, "=2", D5:D300, "=1")</f>
+        <f>AVERAGEIFS(G5:G556, G5:G556, "&gt;0", C5:C556, "=2", D5:D556, "=1")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1506,7 +1506,7 @@
         <v>175</v>
       </c>
       <c r="L23" s="10" t="e">
-        <f>AVERAGEIFS(H5:H300, H5:H300, "&gt;0", C5:C300, "=2", D5:D300, "=1")</f>
+        <f>AVERAGEIFS(H5:H556, H5:H556, "&gt;0", C5:C556, "=2", D5:D556, "=1")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1523,7 +1523,7 @@
         <v>174</v>
       </c>
       <c r="L24" s="10" t="e">
-        <f>AVERAGEIFS(I5:I300, I5:I300, "&gt;0", C5:C300, "=2", D5:D300, "=1")</f>
+        <f>AVERAGEIFS(I5:I556, I5:I556, "&gt;0", C5:C556, "=2", D5:D556, "=1")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1540,7 +1540,7 @@
         <v>158</v>
       </c>
       <c r="L25" s="10" t="e">
-        <f>AVERAGEIFS(F5:F300, F5:F300, "&gt;0", C5:C300, "=1", D5:D300, "=2")</f>
+        <f>AVERAGEIFS(F5:F556, F5:F556, "&gt;0", C5:C556, "=1", D5:D556, "=2")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1557,7 +1557,7 @@
         <v>159</v>
       </c>
       <c r="L26" s="10" t="e">
-        <f>AVERAGEIFS(G5:G300, G5:G300, "&gt;0", C5:C300, "=1", D5:D300, "=2")</f>
+        <f>AVERAGEIFS(G5:G556, G5:G556, "&gt;0", C5:C556, "=1", D5:D556, "=2")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1574,7 +1574,7 @@
         <v>160</v>
       </c>
       <c r="L27" s="10" t="e">
-        <f>AVERAGEIFS(H5:H300, H5:H300, "&gt;0", C5:C300, "=1", D5:D300, "=2")</f>
+        <f>AVERAGEIFS(H5:H556, H5:H556, "&gt;0", C5:C556, "=1", D5:D556, "=2")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
         <v>161</v>
       </c>
       <c r="L28" s="10" t="e">
-        <f>AVERAGEIFS(I5:I300, I5:I300, "&gt;0", C5:C300, "=1", D5:D300, "=2")</f>
+        <f>AVERAGEIFS(I5:I556, I5:I556, "&gt;0", C5:C556, "=1", D5:D556, "=2")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1608,7 +1608,7 @@
         <v>173</v>
       </c>
       <c r="L29" s="10" t="e">
-        <f>AVERAGEIFS(F5:F300, F5:F300, "&gt;0", C5:C300, "=2", D5:D300, "=2")</f>
+        <f>AVERAGEIFS(F5:F556, F5:F556, "&gt;0", C5:C556, "=2", D5:D556, "=2")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1625,7 +1625,7 @@
         <v>172</v>
       </c>
       <c r="L30" s="10" t="e">
-        <f>AVERAGEIFS(G5:G300, G5:G300, "&gt;0", C5:C300, "=2", D5:D300, "=2")</f>
+        <f>AVERAGEIFS(G5:G556, G5:G556, "&gt;0", C5:C556, "=2", D5:D556, "=2")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
         <v>171</v>
       </c>
       <c r="L31" s="10" t="e">
-        <f>AVERAGEIFS(H5:H300, H5:H300, "&gt;0", C5:C300, "=2", D5:D300, "=2")</f>
+        <f>AVERAGEIFS(H5:H556, H5:H556, "&gt;0", C5:C556, "=2", D5:D556, "=2")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1659,7 +1659,7 @@
         <v>170</v>
       </c>
       <c r="L32" s="10" t="e">
-        <f>AVERAGEIFS(I5:I300, I5:I300, "&gt;0", C5:C300, "=2", D5:D300, "=2")</f>
+        <f>AVERAGEIFS(I5:I556, I5:I556, "&gt;0", C5:C556, "=2", D5:D556, "=2")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1676,7 +1676,7 @@
         <v>162</v>
       </c>
       <c r="L33" s="10" t="e">
-        <f>AVERAGEIFS(F5:F300, F5:F300, "&gt;0", C5:C300, "=1", D5:D300, "=3")</f>
+        <f>AVERAGEIFS(F5:F556, F5:F556, "&gt;0", C5:C556, "=1", D5:D556, "=3")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1693,7 +1693,7 @@
         <v>163</v>
       </c>
       <c r="L34" s="10" t="e">
-        <f>AVERAGEIFS(G5:G300, G5:G300, "&gt;0", C5:C300, "=1", D5:D300, "=3")</f>
+        <f>AVERAGEIFS(G5:G556, G5:G556, "&gt;0", C5:C556, "=1", D5:D556, "=3")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1710,7 +1710,7 @@
         <v>164</v>
       </c>
       <c r="L35" s="10" t="e">
-        <f>AVERAGEIFS(H5:H300, H5:H300, "&gt;0", C5:C300, "=1", D5:D300, "=3")</f>
+        <f>AVERAGEIFS(H5:H556, H5:H556, "&gt;0", C5:C556, "=1", D5:D556, "=3")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
         <v>165</v>
       </c>
       <c r="L36" s="10" t="e">
-        <f>AVERAGEIFS(I5:I300, I5:I300, "&gt;0", C5:C300, "=1", D5:D300, "=3")</f>
+        <f>AVERAGEIFS(I5:I556, I5:I556, "&gt;0", C5:C556, "=1", D5:D556, "=3")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1744,7 +1744,7 @@
         <v>169</v>
       </c>
       <c r="L37" s="10" t="e">
-        <f>AVERAGEIFS(F5:F300, F5:F300, "&gt;0", C5:C300, "=2", D5:D300, "=3")</f>
+        <f>AVERAGEIFS(F5:F556, F5:F556, "&gt;0", C5:C556, "=2", D5:D556, "=3")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
         <v>168</v>
       </c>
       <c r="L38" s="10" t="e">
-        <f>AVERAGEIFS(G5:G300, G5:G300, "&gt;0", C5:C300, "=2", D5:D300, "=3")</f>
+        <f>AVERAGEIFS(G5:G556, G5:G556, "&gt;0", C5:C556, "=2", D5:D556, "=3")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1778,7 +1778,7 @@
         <v>167</v>
       </c>
       <c r="L39" s="10" t="e">
-        <f>AVERAGEIFS(H5:H300, H5:H300, "&gt;0", C5:C300, "=2", D5:D300, "=3")</f>
+        <f>AVERAGEIFS(H5:H556, H5:H556, "&gt;0", C5:C556, "=2", D5:D556, "=3")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1795,7 +1795,7 @@
         <v>166</v>
       </c>
       <c r="L40" s="10" t="e">
-        <f>AVERAGEIFS(I5:I300, I5:I300, "&gt;0", C5:C300, "=2", D5:D300, "=3")</f>
+        <f>AVERAGEIFS(I5:I556, I5:I556, "&gt;0", C5:C556, "=2", D5:D556, "=3")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3861,7 +3861,7 @@
   <dimension ref="A1:S565"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="M5" sqref="M5:M130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>